<commit_message>
Move raw data in folder
</commit_message>
<xml_diff>
--- a/Result/Data_Fig3.xlsx
+++ b/Result/Data_Fig3.xlsx
@@ -1,28 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jean-loup-faulon/Desktop/AMN/amn/Result/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faure\Documents\GitHub\amn_release\Result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{0CA365C8-C8C5-0048-B331-898D24C19B2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{586DC024-5A57-4455-BF39-FD18A1ABC682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Fig4" sheetId="2" r:id="rId1"/>
+    <sheet name="Fig3" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -110,7 +113,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -622,58 +625,57 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
     <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Avertissement" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Calcul" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Cellule liée" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Entrée" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Insatisfaisant" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Neutre" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Satisfaisant" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Sortie" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texte explicatif" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Titre" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Titre 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Titre 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Titre 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Titre 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Vérification" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -689,7 +691,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -984,16 +986,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="V28" sqref="V28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1043,7 +1045,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0.16958846599999999</v>
       </c>
@@ -1102,7 +1104,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0.13401355600000001</v>
       </c>
@@ -1158,7 +1160,7 @@
         <v>2.2119663831372937E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.18857015999999999</v>
       </c>
@@ -1213,12 +1215,12 @@
         <f t="shared" si="5"/>
         <v>1.9994721492546115E-2</v>
       </c>
-      <c r="R4" s="4" t="s">
+      <c r="R4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="S4" s="4"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S4" s="3"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.19897683299999999</v>
       </c>
@@ -1273,14 +1275,14 @@
         <f t="shared" si="5"/>
         <v>3.733859403758177E-3</v>
       </c>
-      <c r="R5" s="2" t="s">
+      <c r="R5" t="s">
         <v>17</v>
       </c>
-      <c r="S5" s="2">
+      <c r="S5">
         <v>0.88040289292450313</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>7.1987774000000004E-2</v>
       </c>
@@ -1335,14 +1337,14 @@
         <f t="shared" si="5"/>
         <v>8.2180858597920257E-3</v>
       </c>
-      <c r="R6" s="2" t="s">
+      <c r="R6" t="s">
         <v>18</v>
       </c>
-      <c r="S6" s="2">
+      <c r="S6">
         <v>0.7751092538698342</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>9.2418342000000001E-2</v>
       </c>
@@ -1397,14 +1399,14 @@
         <f t="shared" si="5"/>
         <v>7.722316732046897E-3</v>
       </c>
-      <c r="R7" s="2" t="s">
+      <c r="R7" t="s">
         <v>19</v>
       </c>
-      <c r="S7" s="2">
+      <c r="S7">
         <v>0.77302693214640683</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8.8127767999999995E-2</v>
       </c>
@@ -1459,14 +1461,14 @@
         <f t="shared" si="5"/>
         <v>2.5648007886875029E-2</v>
       </c>
-      <c r="R8" s="2" t="s">
+      <c r="R8" t="s">
         <v>20</v>
       </c>
-      <c r="S8" s="2">
+      <c r="S8">
         <v>3.5321589521430566E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8.9982767000000005E-2</v>
       </c>
@@ -1521,14 +1523,14 @@
         <f t="shared" si="5"/>
         <v>2.345866362423941E-3</v>
       </c>
-      <c r="R9" s="3" t="s">
+      <c r="R9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="S9" s="3">
+      <c r="S9" s="2">
         <v>110</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.198852586</v>
       </c>
@@ -1584,7 +1586,7 @@
         <v>1.3149174926585547E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0.105387655</v>
       </c>
@@ -1640,7 +1642,7 @@
         <v>2.6914579073469894E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0.26806338800000001</v>
       </c>
@@ -1699,7 +1701,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>0.15756536099999999</v>
       </c>
@@ -1755,7 +1757,7 @@
         <v>1.3020143585633427E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0.120922381</v>
       </c>
@@ -1810,12 +1812,12 @@
         <f t="shared" si="5"/>
         <v>2.1819422318940636E-2</v>
       </c>
-      <c r="R14" s="4" t="s">
+      <c r="R14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="S14" s="4"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S14" s="3"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0.27287330799999998</v>
       </c>
@@ -1870,14 +1872,14 @@
         <f t="shared" si="5"/>
         <v>1.1811584343584362E-2</v>
       </c>
-      <c r="R15" s="2" t="s">
+      <c r="R15" t="s">
         <v>17</v>
       </c>
-      <c r="S15" s="2">
+      <c r="S15">
         <v>0.94081361841770084</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0.29449713799999999</v>
       </c>
@@ -1932,14 +1934,14 @@
         <f t="shared" si="5"/>
         <v>3.9196741986321608E-3</v>
       </c>
-      <c r="R16" s="2" t="s">
+      <c r="R16" t="s">
         <v>18</v>
       </c>
-      <c r="S16" s="2">
+      <c r="S16">
         <v>0.88513026460020716</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0.238556665</v>
       </c>
@@ -1994,14 +1996,14 @@
         <f t="shared" si="5"/>
         <v>1.2142500637196227E-2</v>
       </c>
-      <c r="R17" s="2" t="s">
+      <c r="R17" t="s">
         <v>19</v>
       </c>
-      <c r="S17" s="2">
+      <c r="S17">
         <v>0.88406665593909806</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0.25305511200000003</v>
       </c>
@@ -2056,14 +2058,14 @@
         <f t="shared" si="5"/>
         <v>3.2273152157808752E-2</v>
       </c>
-      <c r="R18" s="2" t="s">
+      <c r="R18" t="s">
         <v>20</v>
       </c>
-      <c r="S18" s="2">
+      <c r="S18">
         <v>2.5243946836655165E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>0.26057602600000002</v>
       </c>
@@ -2118,14 +2120,14 @@
         <f t="shared" si="5"/>
         <v>8.7684883094472296E-3</v>
       </c>
-      <c r="R19" s="3" t="s">
+      <c r="R19" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="S19" s="3">
+      <c r="S19" s="2">
         <v>110</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>0.28162630700000002</v>
       </c>
@@ -2181,7 +2183,7 @@
         <v>1.3133076665131199E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0.135054594</v>
       </c>
@@ -2237,7 +2239,7 @@
         <v>1.2084538397159705E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0.14489148900000001</v>
       </c>
@@ -2296,7 +2298,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>0.24085268000000001</v>
       </c>
@@ -2352,7 +2354,7 @@
         <v>7.6885694829330947E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0.24372696899999999</v>
       </c>
@@ -2407,12 +2409,12 @@
         <f t="shared" si="5"/>
         <v>1.6929915724884292E-2</v>
       </c>
-      <c r="R24" s="4" t="s">
+      <c r="R24" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="S24" s="4"/>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S24" s="3"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0.105929867</v>
       </c>
@@ -2467,14 +2469,14 @@
         <f t="shared" si="5"/>
         <v>2.1491205138165714E-2</v>
       </c>
-      <c r="R25" s="2" t="s">
+      <c r="R25" t="s">
         <v>17</v>
       </c>
-      <c r="S25" s="2">
+      <c r="S25">
         <v>0.94342681504989134</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0.108236991</v>
       </c>
@@ -2529,14 +2531,14 @@
         <f t="shared" si="5"/>
         <v>2.331766987294874E-2</v>
       </c>
-      <c r="R26" s="2" t="s">
+      <c r="R26" t="s">
         <v>18</v>
       </c>
-      <c r="S26" s="2">
+      <c r="S26">
         <v>0.89005415535518195</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>0.24511303100000001</v>
       </c>
@@ -2591,14 +2593,14 @@
         <f t="shared" si="5"/>
         <v>2.377684712369545E-2</v>
       </c>
-      <c r="R27" s="2" t="s">
+      <c r="R27" t="s">
         <v>19</v>
       </c>
-      <c r="S27" s="2">
+      <c r="S27">
         <v>0.88903613827513728</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>0.30990109300000002</v>
       </c>
@@ -2653,14 +2655,14 @@
         <f t="shared" si="5"/>
         <v>1.0082179755943435E-2</v>
       </c>
-      <c r="R28" s="2" t="s">
+      <c r="R28" t="s">
         <v>20</v>
       </c>
-      <c r="S28" s="2">
+      <c r="S28">
         <v>2.4696980371054771E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>0.199950031</v>
       </c>
@@ -2715,14 +2717,14 @@
         <f t="shared" si="5"/>
         <v>1.329358345211543E-2</v>
       </c>
-      <c r="R29" s="3" t="s">
+      <c r="R29" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="S29" s="3">
+      <c r="S29" s="2">
         <v>110</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>0.207729257</v>
       </c>
@@ -2778,7 +2780,7 @@
         <v>1.1103423405374502E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>0.38366266799999998</v>
       </c>
@@ -2834,7 +2836,7 @@
         <v>1.5927783933795563E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>0.22467949500000001</v>
       </c>
@@ -2890,7 +2892,7 @@
         <v>1.2120006000242408E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>0.35197431099999998</v>
       </c>
@@ -2946,7 +2948,7 @@
         <v>9.9445997436684152E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>0.22554864399999999</v>
       </c>
@@ -3002,7 +3004,7 @@
         <v>5.4949410793475187E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>0.13398423400000001</v>
       </c>
@@ -3058,7 +3060,7 @@
         <v>1.6594500953945428E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>0.23969573499999999</v>
       </c>
@@ -3114,7 +3116,7 @@
         <v>1.2175285716946576E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>0.36538323</v>
       </c>
@@ -3170,7 +3172,7 @@
         <v>5.7138564445940399E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>0.18627597400000001</v>
       </c>
@@ -3226,7 +3228,7 @@
         <v>3.1375112548490798E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>0.16118613300000001</v>
       </c>
@@ -3282,7 +3284,7 @@
         <v>2.755774883581328E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>0.344171114</v>
       </c>
@@ -3338,7 +3340,7 @@
         <v>9.3694667982559168E-4</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>0.29636433600000001</v>
       </c>
@@ -3394,7 +3396,7 @@
         <v>1.3600676012258695E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>0.41345673700000002</v>
       </c>
@@ -3450,7 +3452,7 @@
         <v>2.7095673594553199E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>0.25608325100000001</v>
       </c>
@@ -3506,7 +3508,7 @@
         <v>1.3463086841846092E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>0.39489685800000002</v>
       </c>
@@ -3562,7 +3564,7 @@
         <v>3.3787830315040825E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>0.42053847599999999</v>
       </c>
@@ -3618,7 +3620,7 @@
         <v>1.8338287606508141E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>0.30498804899999998</v>
       </c>
@@ -3674,7 +3676,7 @@
         <v>2.9959026105020631E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>0.23150512000000001</v>
       </c>
@@ -3730,7 +3732,7 @@
         <v>1.3779067115813075E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>0.27081595600000002</v>
       </c>
@@ -3786,7 +3788,7 @@
         <v>1.9373939275025547E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>0.33509877599999999</v>
       </c>
@@ -3842,7 +3844,7 @@
         <v>2.2053625208042389E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>0.27848960699999997</v>
       </c>
@@ -3898,7 +3900,7 @@
         <v>1.7606112830305228E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>7.6529395E-2</v>
       </c>
@@ -3954,7 +3956,7 @@
         <v>2.1954057420480014E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>7.0366423999999997E-2</v>
       </c>
@@ -4010,7 +4012,7 @@
         <v>1.0677867668869464E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>0.20953582700000001</v>
       </c>
@@ -4066,7 +4068,7 @@
         <v>1.4256219364695609E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>0.11354415900000001</v>
       </c>
@@ -4122,7 +4124,7 @@
         <v>8.2139402362363303E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>0.21931910499999999</v>
       </c>
@@ -4178,7 +4180,7 @@
         <v>1.6930989502024599E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>0.33156463899999999</v>
       </c>
@@ -4234,7 +4236,7 @@
         <v>1.4455499697146055E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>0.13677539499999999</v>
       </c>
@@ -4290,7 +4292,7 @@
         <v>2.3191860621577128E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>0.13622546999999999</v>
       </c>
@@ -4346,7 +4348,7 @@
         <v>9.6182566853214094E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>0.10738262</v>
       </c>
@@ -4402,7 +4404,7 @@
         <v>2.6563372265190738E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>0.22768200699999999</v>
       </c>
@@ -4458,7 +4460,7 @@
         <v>1.4827173169345974E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>0.20206659900000001</v>
       </c>
@@ -4514,7 +4516,7 @@
         <v>2.6934697006667282E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>0.227544843</v>
       </c>
@@ -4570,7 +4572,7 @@
         <v>3.5931396673731129E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>0.21310800099999999</v>
       </c>
@@ -4626,7 +4628,7 @@
         <v>4.4054712699550004E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>0.26244328099999997</v>
       </c>
@@ -4682,7 +4684,7 @@
         <v>6.1612967360962891E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>0.18620894900000001</v>
       </c>
@@ -4738,7 +4740,7 @@
         <v>1.399148101710484E-4</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>0.16876882900000001</v>
       </c>
@@ -4794,7 +4796,7 @@
         <v>3.3256034039183271E-3</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>0.36209366599999998</v>
       </c>
@@ -4850,7 +4852,7 @@
         <v>1.2849967159395285E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>0.25491721099999998</v>
       </c>
@@ -4906,7 +4908,7 @@
         <v>7.2539112513194887E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>0.242919828</v>
       </c>
@@ -4962,7 +4964,7 @@
         <v>1.2240857684355812E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>0.19361131400000001</v>
       </c>
@@ -5018,7 +5020,7 @@
         <v>6.0258806631804263E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>0.33610418600000003</v>
       </c>
@@ -5074,7 +5076,7 @@
         <v>2.4991927243909525E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>0.36883461499999998</v>
       </c>
@@ -5130,7 +5132,7 @@
         <v>2.4991297513955279E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>0.17652818300000001</v>
       </c>
@@ -5186,7 +5188,7 @@
         <v>9.5299900921871107E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>0.158459452</v>
       </c>
@@ -5242,7 +5244,7 @@
         <v>1.0419586746150492E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>0.15383750199999999</v>
       </c>
@@ -5298,7 +5300,7 @@
         <v>5.8817357257281043E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>0.18870321100000001</v>
       </c>
@@ -5354,7 +5356,7 @@
         <v>4.9546702216466346E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>0.16546936400000001</v>
       </c>
@@ -5410,7 +5412,7 @@
         <v>1.0169478486246473E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>0.17060508399999999</v>
       </c>
@@ -5466,7 +5468,7 @@
         <v>3.1673320055461383E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>0.21547613400000001</v>
       </c>
@@ -5522,7 +5524,7 @@
         <v>8.46463875875186E-3</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>0.15491189299999999</v>
       </c>
@@ -5578,7 +5580,7 @@
         <v>1.1251047078005685E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>0.30221964299999998</v>
       </c>
@@ -5634,7 +5636,7 @@
         <v>5.4911454729875625E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>0.27056665299999999</v>
       </c>
@@ -5690,7 +5692,7 @@
         <v>1.8748805454224901E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>0.240512226</v>
       </c>
@@ -5746,7 +5748,7 @@
         <v>6.0846940135901939E-3</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>0.33618462500000001</v>
       </c>
@@ -5802,7 +5804,7 @@
         <v>2.6215807996959124E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>0.302654535</v>
       </c>
@@ -5858,7 +5860,7 @@
         <v>9.0061939875151521E-3</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>0.19236412999999999</v>
       </c>
@@ -5914,7 +5916,7 @@
         <v>8.6488191366726353E-3</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>0.167390027</v>
       </c>
@@ -5970,7 +5972,7 @@
         <v>2.1646019740976317E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>0.32553523000000001</v>
       </c>
@@ -6026,7 +6028,7 @@
         <v>2.5961627091550827E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>0.25188356499999998</v>
       </c>
@@ -6082,7 +6084,7 @@
         <v>1.2745686470261832E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>0.335468814</v>
       </c>
@@ -6138,7 +6140,7 @@
         <v>2.5204334246139656E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>0.29190892699999998</v>
       </c>
@@ -6194,7 +6196,7 @@
         <v>1.5499836293567441E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>0.30484687799999999</v>
       </c>
@@ -6250,7 +6252,7 @@
         <v>1.5709442427931646E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>0.23701744599999999</v>
       </c>
@@ -6306,7 +6308,7 @@
         <v>1.9202241454729457E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>0.29771937399999998</v>
       </c>
@@ -6362,7 +6364,7 @@
         <v>1.9050055788744844E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>0.246085944</v>
       </c>
@@ -6418,7 +6420,7 @@
         <v>5.6049300660018231E-3</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>0.23097748600000001</v>
       </c>
@@ -6474,7 +6476,7 @@
         <v>1.2653681112952297E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>0.203747447</v>
       </c>
@@ -6530,7 +6532,7 @@
         <v>1.4094666721996796E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>0.34018670600000001</v>
       </c>
@@ -6586,7 +6588,7 @@
         <v>7.028508411943084E-3</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>0.20408690600000001</v>
       </c>
@@ -6642,7 +6644,7 @@
         <v>1.6439453191945147E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>0.166473868</v>
       </c>
@@ -6698,7 +6700,7 @@
         <v>1.7465458572881665E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>0.131987304</v>
       </c>
@@ -6754,7 +6756,7 @@
         <v>6.5089829396008814E-3</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>0.27311799399999998</v>
       </c>
@@ -6810,7 +6812,7 @@
         <v>7.0716348456610926E-3</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>0.37845480999999997</v>
       </c>
@@ -6866,7 +6868,7 @@
         <v>4.9032855871392431E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>0.23210631000000001</v>
       </c>
@@ -6922,7 +6924,7 @@
         <v>1.2079568325644366E-2</v>
       </c>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>0.36748529400000002</v>
       </c>
@@ -6978,7 +6980,7 @@
         <v>1.5491295599266682E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>0.27124000700000001</v>
       </c>
@@ -7034,7 +7036,7 @@
         <v>9.0551033827776396E-3</v>
       </c>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>0.26096545500000001</v>
       </c>
@@ -7090,7 +7092,7 @@
         <v>8.3933754773464382E-3</v>
       </c>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>0.24690668499999999</v>
       </c>
@@ -7146,7 +7148,7 @@
         <v>8.5197297753879363E-3</v>
       </c>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>0.39292908599999998</v>
       </c>
@@ -7202,7 +7204,7 @@
         <v>1.6563025198695489E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>0.36302644699999997</v>
       </c>
@@ -7258,7 +7260,7 @@
         <v>2.4157196208544934E-2</v>
       </c>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>0.19488303900000001</v>
       </c>

</xml_diff>